<commit_message>
[Workinng version of display reciepe]
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ReciepeType</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>1. Heat the milk in a broad non-stick pan and cook on a medium flame for 5 to 6 minutes or till it starts boiling, while stirring occasionally. 2. Keep aside to cool completely. 3. Once cooled, add the sugar substitute and cardamom powder and mix well.4. Add the 5. Serve chilled.paneer and mix well. Refrigerate for at least 1 hour.</t>
+  </si>
+  <si>
+    <t>ReciepeID</t>
+  </si>
+  <si>
+    <t>Desert</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +449,7 @@
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +483,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -506,8 +515,11 @@
       <c r="I2" t="b">
         <v>0</v>
       </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -535,11 +547,17 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
@@ -560,6 +578,9 @@
       </c>
       <c r="I4" t="b">
         <v>1</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Works with css and images
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ReciepeType</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Desert</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>TomatoCurry.jpg</t>
+  </si>
+  <si>
+    <t>Brinjal-rice.jpg</t>
+  </si>
+  <si>
+    <t>gajar.jpg</t>
   </si>
 </sst>
 </file>
@@ -430,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +461,7 @@
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,8 +498,11 @@
       <c r="L1" t="s">
         <v>19</v>
       </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,8 +533,11 @@
       <c r="L2">
         <v>1</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -550,8 +568,11 @@
       <c r="L3">
         <v>2</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -581,6 +602,9 @@
       </c>
       <c r="L4">
         <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Working Model with Background]
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>ReciepeType</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>gajar.jpg</t>
+  </si>
+  <si>
+    <t>PotatoCurry</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +462,7 @@
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -605,6 +609,38 @@
       </c>
       <c r="M4" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>